<commit_message>
Cambios de los procesos
</commit_message>
<xml_diff>
--- a/Data/template/Machote de CIISA - Copy - Copy.xlsx
+++ b/Data/template/Machote de CIISA - Copy - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\walner.borbon\OneDrive - Grant Thornton CR\Documents\UiPath\CIISA-Bot\Data\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8252947E-6411-446F-A254-E8327450AC5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4259E95A-7FBC-4749-A513-86BC74645351}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="690" yWindow="690" windowWidth="14205" windowHeight="12750" tabRatio="602" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="detalle ajustado" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId3"/>
+    <pivotCache cacheId="8" r:id="rId3"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -5219,7 +5219,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000001000000}" name="TablaDinámica2" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000001000000}" name="TablaDinámica2" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A12:F18" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField showAll="0"/>
@@ -5320,7 +5320,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="TablaDinámica1" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="TablaDinámica1" cacheId="8" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Valores" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A3:F6" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="17">
     <pivotField showAll="0"/>
@@ -5708,7 +5708,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:S784"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="L765" workbookViewId="0">
       <selection activeCell="P784" sqref="N3:P784"/>
     </sheetView>
   </sheetViews>
@@ -28354,7 +28354,7 @@
         <v>11</v>
       </c>
       <c r="P784" s="7" t="str">
-        <f t="shared" ref="P784" si="67">IF(D784="ropa, zapateria y hogar","otros",IF(D784="otros","taxi",IF(D784="restaurantes","Alimentacion",IF(D784="hoteles","hospedaje",IF(D784="supermercados","Alimentacion",IF(D784="agencia de viajes","viajes exterior",IF(D784="aerolineas","viajes exterior","incorrecto")))))))</f>
+        <f>IF(D784="ropa, zapateria y hogar","COMPRAS MENORES(**)",IF(D784="otros","taxi",IF(D784="restaurantes","Alimentacion",IF(D784="hoteles","hospedaje",IF(D784="supermercados","Alimentacion",IF(D784="agencia de viajes","viajes exterior",IF(D784="aerolineas","viajes exterior","incorrecto")))))))</f>
         <v>incorrecto</v>
       </c>
       <c r="Q784" s="5">

</xml_diff>